<commit_message>
added a draft for scene based simulations rather than individual based ones
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios.xlsx
+++ b/test/inputs/Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D26BAFC-DA2D-4C18-811E-D9712B5343D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7713F94E-2565-4F75-8F5B-6CDC2B0155D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="496">
   <si>
     <t>input_file</t>
   </si>
@@ -1513,6 +1513,15 @@
   </si>
   <si>
     <t>roots</t>
+  </si>
+  <si>
+    <t>xylem_cross_area_ratio</t>
+  </si>
+  <si>
+    <t>apoplasmic cross-section area ratio * stele radius ratio^2</t>
+  </si>
+  <si>
+    <t>adim</t>
   </si>
 </sst>
 </file>
@@ -2168,7 +2177,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2368,6 +2377,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2689,10 +2709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J200"/>
+  <dimension ref="A1:J201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="H192" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="H182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="I207" sqref="I207"/>
@@ -8687,32 +8707,63 @@
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="1" t="s">
+      <c r="A200" s="97" t="s">
+        <v>493</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="C200" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D200" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="E200" s="98" t="s">
+        <v>494</v>
+      </c>
+      <c r="F200" s="98" t="s">
+        <v>495</v>
+      </c>
+      <c r="G200" s="99">
+        <f>0.84*(0.36*0.36)</f>
+        <v>0.10886399999999999</v>
+      </c>
+      <c r="H200" s="100">
+        <f>G200</f>
+        <v>0.10886399999999999</v>
+      </c>
+      <c r="I200" s="101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A201" s="1" t="s">
         <v>485</v>
       </c>
-      <c r="B200" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C200" s="1" t="s">
+      <c r="B201" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="C201" s="1" t="s">
         <v>486</v>
       </c>
-      <c r="D200" s="1" t="s">
+      <c r="D201" s="1" t="s">
         <v>492</v>
       </c>
-      <c r="E200" s="94" t="s">
+      <c r="E201" s="94" t="s">
         <v>487</v>
       </c>
-      <c r="F200" s="94" t="s">
+      <c r="F201" s="94" t="s">
         <v>488</v>
       </c>
-      <c r="G200" s="95">
+      <c r="G201" s="95">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="H200" s="95">
-        <f>G200</f>
+      <c r="H201" s="95">
+        <f>G201</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="I200" s="96">
+      <c r="I201" s="96">
         <v>9.9999999999999995E-8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
spotted mistakes in unit conversion in coupling_translator
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios.xlsx
+++ b/test/inputs/Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7713F94E-2565-4F75-8F5B-6CDC2B0155D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3A93A1-5E6F-41AA-8E52-7088782B1C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2377,15 +2377,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2715,7 +2715,7 @@
       <pane xSplit="7" ySplit="4" topLeftCell="H182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I207" sqref="I207"/>
+      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8734,7 +8734,7 @@
         <v>0.10886399999999999</v>
       </c>
       <c r="I200" s="101">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Transfered cnwheat collar modification to a separate file for the sake of modularity
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios.xlsx
+++ b/test/inputs/Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3A93A1-5E6F-41AA-8E52-7088782B1C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49A5DB2-7BEC-41C2-B679-FE495122B356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2715,7 +2715,7 @@
       <pane xSplit="7" ySplit="4" topLeftCell="H182" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I201" sqref="I201"/>
+      <selection pane="bottomRight" activeCell="E215" sqref="E215"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8734,7 +8734,8 @@
         <v>0.10886399999999999</v>
       </c>
       <c r="I200" s="101">
-        <v>10</v>
+        <f>H200</f>
+        <v>0.10886399999999999</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
mutliprocessing simulations when to test parametrization
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios.xlsx
+++ b/test/inputs/Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D49A5DB2-7BEC-41C2-B679-FE495122B356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEF4D05-677F-4FC0-84BF-13A727FAB37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1598" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1658" uniqueCount="498">
   <si>
     <t>input_file</t>
   </si>
@@ -1522,6 +1522,12 @@
   </si>
   <si>
     <t>adim</t>
+  </si>
+  <si>
+    <t>WB2</t>
+  </si>
+  <si>
+    <t>WB3</t>
   </si>
 </sst>
 </file>
@@ -1991,7 +1997,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2132,6 +2138,19 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -2177,7 +2196,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2373,21 +2392,24 @@
     </xf>
     <xf numFmtId="165" fontId="16" fillId="51" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="46" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="11" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="16" fillId="50" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2709,13 +2731,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J201"/>
+  <dimension ref="A1:L201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="H182" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="H185" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E215" sqref="E215"/>
+      <selection pane="bottomRight" activeCell="J213" sqref="J213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2728,10 +2750,10 @@
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" style="40" customWidth="1"/>
     <col min="8" max="8" width="45" style="40" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" style="1" customWidth="1"/>
+    <col min="9" max="11" width="21.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>472</v>
       </c>
@@ -2759,8 +2781,14 @@
       <c r="I1" s="38" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J1" s="38" t="s">
+        <v>496</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>483</v>
       </c>
@@ -2789,8 +2817,16 @@
       <c r="I2" s="80" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J2" s="80" t="str">
+        <f>I2</f>
+        <v>root_3_leaves.pckl</v>
+      </c>
+      <c r="K2" s="80" t="str">
+        <f>J2</f>
+        <v>root_3_leaves.pckl</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>480</v>
       </c>
@@ -2818,8 +2854,14 @@
       <c r="I3" s="1" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="1" t="s">
+        <v>477</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -2848,8 +2890,14 @@
       <c r="I4" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K4" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
@@ -2878,8 +2926,14 @@
       <c r="I5" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="80">
+        <v>1</v>
+      </c>
+      <c r="K5" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -2908,8 +2962,14 @@
       <c r="I6" s="89">
         <v>180</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="89">
+        <v>180</v>
+      </c>
+      <c r="K6" s="89">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -2938,8 +2998,14 @@
       <c r="I7" s="81">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="81">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="K7" s="81">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>20</v>
       </c>
@@ -2968,8 +3034,14 @@
       <c r="I8" s="82">
         <v>4.1666666999999998E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="82">
+        <v>4.1666666999999998E-2</v>
+      </c>
+      <c r="K8" s="82">
+        <v>4.1666666999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>1</v>
       </c>
@@ -2998,8 +3070,14 @@
       <c r="I9" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="80">
+        <v>1</v>
+      </c>
+      <c r="K9" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>450</v>
       </c>
@@ -3028,8 +3106,14 @@
       <c r="I10" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="80">
+        <v>0</v>
+      </c>
+      <c r="K10" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>6</v>
       </c>
@@ -3058,8 +3142,14 @@
       <c r="I11" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K11" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
@@ -3088,8 +3178,14 @@
       <c r="I12" s="83">
         <v>5.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="83">
+        <v>5.0000000000000001E-9</v>
+      </c>
+      <c r="K12" s="83">
+        <v>5.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
         <v>8</v>
       </c>
@@ -3118,8 +3214,14 @@
       <c r="I13" s="80">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="80">
+        <v>10</v>
+      </c>
+      <c r="K13" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>463</v>
       </c>
@@ -3148,8 +3250,14 @@
       <c r="I14" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K14" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>464</v>
       </c>
@@ -3178,8 +3286,14 @@
       <c r="I15" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K15" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>467</v>
       </c>
@@ -3208,8 +3322,14 @@
       <c r="I16" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K16" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>469</v>
       </c>
@@ -3238,8 +3358,14 @@
       <c r="I17" s="80">
         <v>86400</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="80">
+        <v>86400</v>
+      </c>
+      <c r="K17" s="80">
+        <v>86400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>10</v>
       </c>
@@ -3268,8 +3394,14 @@
       <c r="I18" s="89" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="89" t="s">
+        <v>87</v>
+      </c>
+      <c r="K18" s="89" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>11</v>
       </c>
@@ -3298,8 +3430,14 @@
       <c r="I19" s="80">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="80">
+        <v>3</v>
+      </c>
+      <c r="K19" s="80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>362</v>
       </c>
@@ -3328,8 +3466,14 @@
       <c r="I20" s="84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="K20" s="84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>364</v>
       </c>
@@ -3358,8 +3502,14 @@
       <c r="I21" s="84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="K21" s="84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>376</v>
       </c>
@@ -3388,8 +3538,14 @@
       <c r="I22" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K22" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>375</v>
       </c>
@@ -3418,8 +3574,14 @@
       <c r="I23" s="84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="K23" s="84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>374</v>
       </c>
@@ -3448,8 +3610,14 @@
       <c r="I24" s="84" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="K24" s="84" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>12</v>
       </c>
@@ -3478,8 +3646,14 @@
       <c r="I25" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K25" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
         <v>13</v>
       </c>
@@ -3508,8 +3682,14 @@
       <c r="I26" s="80">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="80">
+        <v>0.33</v>
+      </c>
+      <c r="K26" s="80">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
         <v>14</v>
       </c>
@@ -3538,8 +3718,14 @@
       <c r="I27" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K27" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
         <v>9</v>
       </c>
@@ -3568,8 +3754,14 @@
       <c r="I28" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K28" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
         <v>456</v>
       </c>
@@ -3598,8 +3790,14 @@
       <c r="I29" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K29" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="13" t="s">
         <v>21</v>
       </c>
@@ -3628,8 +3826,14 @@
       <c r="I30" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J30" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K30" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>22</v>
       </c>
@@ -3658,8 +3862,14 @@
       <c r="I31" s="89" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J31" s="89" t="s">
+        <v>436</v>
+      </c>
+      <c r="K31" s="89" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>23</v>
       </c>
@@ -3688,8 +3898,14 @@
       <c r="I32" s="83">
         <v>9.9999999999999995E-7</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32" s="83">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="K32" s="83">
+        <v>9.9999999999999995E-7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>24</v>
       </c>
@@ -3718,8 +3934,14 @@
       <c r="I33" s="90">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J33" s="90">
+        <v>1E-3</v>
+      </c>
+      <c r="K33" s="90">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>25</v>
       </c>
@@ -3748,8 +3970,14 @@
       <c r="I34" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K34" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="13" t="s">
         <v>26</v>
       </c>
@@ -3778,8 +4006,14 @@
       <c r="I35" s="80" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J35" s="80" t="s">
+        <v>88</v>
+      </c>
+      <c r="K35" s="80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="13" t="s">
         <v>27</v>
       </c>
@@ -3808,8 +4042,14 @@
       <c r="I36" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K36" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="13" t="s">
         <v>28</v>
       </c>
@@ -3838,8 +4078,14 @@
       <c r="I37" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K37" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>29</v>
       </c>
@@ -3868,8 +4114,14 @@
       <c r="I38" s="80">
         <v>120</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J38" s="80">
+        <v>120</v>
+      </c>
+      <c r="K38" s="80">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="13" t="s">
         <v>30</v>
       </c>
@@ -3898,8 +4150,14 @@
       <c r="I39" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J39" s="80">
+        <v>0</v>
+      </c>
+      <c r="K39" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="13" t="s">
         <v>31</v>
       </c>
@@ -3928,8 +4186,14 @@
       <c r="I40" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40" s="80">
+        <v>0</v>
+      </c>
+      <c r="K40" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>32</v>
       </c>
@@ -3958,8 +4222,14 @@
       <c r="I41" s="80">
         <v>-0.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41" s="80">
+        <v>-0.1</v>
+      </c>
+      <c r="K41" s="80">
+        <v>-0.1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>33</v>
       </c>
@@ -3988,8 +4258,14 @@
       <c r="I42" s="80">
         <v>-0.2</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42" s="80">
+        <v>-0.2</v>
+      </c>
+      <c r="K42" s="80">
+        <v>-0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="13" t="s">
         <v>34</v>
       </c>
@@ -4018,8 +4294,14 @@
       <c r="I43" s="80">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J43" s="80">
+        <v>0.4</v>
+      </c>
+      <c r="K43" s="80">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="13" t="s">
         <v>35</v>
       </c>
@@ -4048,8 +4330,14 @@
       <c r="I44" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J44" s="80">
+        <v>0</v>
+      </c>
+      <c r="K44" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>437</v>
       </c>
@@ -4078,8 +4366,14 @@
       <c r="I45" s="80">
         <v>1200</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J45" s="80">
+        <v>1200</v>
+      </c>
+      <c r="K45" s="80">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="13" t="s">
         <v>438</v>
       </c>
@@ -4108,8 +4402,14 @@
       <c r="I46" s="80">
         <v>1200</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J46" s="80">
+        <v>1200</v>
+      </c>
+      <c r="K46" s="80">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="13" t="s">
         <v>459</v>
       </c>
@@ -4138,8 +4438,14 @@
       <c r="I47" s="37" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J47" s="37" t="s">
+        <v>462</v>
+      </c>
+      <c r="K47" s="37" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="13" t="s">
         <v>15</v>
       </c>
@@ -4168,8 +4474,14 @@
       <c r="I48" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K48" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>16</v>
       </c>
@@ -4198,8 +4510,14 @@
       <c r="I49" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J49" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K49" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>17</v>
       </c>
@@ -4228,8 +4546,14 @@
       <c r="I50" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50" s="80">
+        <v>0</v>
+      </c>
+      <c r="K50" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>18</v>
       </c>
@@ -4258,8 +4582,14 @@
       <c r="I51" s="80">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="K51" s="80">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>19</v>
       </c>
@@ -4288,8 +4618,14 @@
       <c r="I52" s="80">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J52" s="80">
+        <v>0.05</v>
+      </c>
+      <c r="K52" s="80">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="15" t="s">
         <v>36</v>
       </c>
@@ -4318,8 +4654,14 @@
       <c r="I53" s="83">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J53" s="83">
+        <v>1E-3</v>
+      </c>
+      <c r="K53" s="83">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="15" t="s">
         <v>379</v>
       </c>
@@ -4348,8 +4690,14 @@
       <c r="I54" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54" s="80">
+        <v>0</v>
+      </c>
+      <c r="K54" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="15" t="s">
         <v>37</v>
       </c>
@@ -4378,8 +4726,14 @@
       <c r="I55" s="80">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J55" s="80">
+        <v>1E-4</v>
+      </c>
+      <c r="K55" s="80">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="15" t="s">
         <v>38</v>
       </c>
@@ -4408,8 +4762,14 @@
       <c r="I56" s="80">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J56" s="80">
+        <v>1E-4</v>
+      </c>
+      <c r="K56" s="80">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="17" t="s">
         <v>39</v>
       </c>
@@ -4438,8 +4798,14 @@
       <c r="I57" s="80">
         <v>6.9999999999999999E-4</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J57" s="80">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="K57" s="80">
+        <v>6.9999999999999999E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="17" t="s">
         <v>40</v>
       </c>
@@ -4468,8 +4834,14 @@
       <c r="I58" s="80">
         <v>1.22E-4</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J58" s="80">
+        <v>1.22E-4</v>
+      </c>
+      <c r="K58" s="80">
+        <v>1.22E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="17" t="s">
         <v>206</v>
       </c>
@@ -4498,8 +4870,14 @@
       <c r="I59" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J59" s="80">
+        <v>1</v>
+      </c>
+      <c r="K59" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="17" t="s">
         <v>41</v>
       </c>
@@ -4528,8 +4906,14 @@
       <c r="I60" s="80">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J60" s="80">
+        <v>0.95</v>
+      </c>
+      <c r="K60" s="80">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="17" t="s">
         <v>406</v>
       </c>
@@ -4558,8 +4942,14 @@
       <c r="I61" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J61" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K61" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
         <v>90</v>
       </c>
@@ -4588,8 +4978,14 @@
       <c r="I62" s="80">
         <v>5</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J62" s="80">
+        <v>5</v>
+      </c>
+      <c r="K62" s="80">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="17" t="s">
         <v>408</v>
       </c>
@@ -4618,8 +5014,14 @@
       <c r="I63" s="80" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J63" s="80" t="s">
+        <v>87</v>
+      </c>
+      <c r="K63" s="80" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="17" t="s">
         <v>42</v>
       </c>
@@ -4648,8 +5050,14 @@
       <c r="I64" s="80">
         <v>50</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J64" s="80">
+        <v>50</v>
+      </c>
+      <c r="K64" s="80">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
         <v>207</v>
       </c>
@@ -4678,8 +5086,14 @@
       <c r="I65" s="81">
         <v>1453890.8941884842</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J65" s="81">
+        <v>1453890.8941884842</v>
+      </c>
+      <c r="K65" s="81">
+        <v>1453890.8941884842</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
         <v>43</v>
       </c>
@@ -4708,8 +5122,14 @@
       <c r="I66" s="81">
         <v>1.3888888888888888E-5</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66" s="81">
+        <v>1.3888888888888888E-5</v>
+      </c>
+      <c r="K66" s="81">
+        <v>1.3888888888888888E-5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="17" t="s">
         <v>44</v>
       </c>
@@ -4738,8 +5158,14 @@
       <c r="I67" s="82">
         <v>6.5011574074074071E-4</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J67" s="82">
+        <v>6.5011574074074071E-4</v>
+      </c>
+      <c r="K67" s="82">
+        <v>6.5011574074074071E-4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="17" t="s">
         <v>45</v>
       </c>
@@ -4768,8 +5194,14 @@
       <c r="I68" s="89">
         <v>4.7400000000000003E-3</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J68" s="89">
+        <v>4.7400000000000003E-3</v>
+      </c>
+      <c r="K68" s="89">
+        <v>4.7400000000000003E-3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
         <v>46</v>
       </c>
@@ -4798,8 +5230,14 @@
       <c r="I69" s="82">
         <v>282528</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J69" s="82">
+        <v>282528</v>
+      </c>
+      <c r="K69" s="82">
+        <v>282528</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>47</v>
       </c>
@@ -4828,8 +5266,14 @@
       <c r="I70" s="89">
         <v>0.56999999999999995</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J70" s="89">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="K70" s="89">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="17" t="s">
         <v>48</v>
       </c>
@@ -4858,8 +5302,14 @@
       <c r="I71" s="91">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J71" s="91">
+        <v>0.16</v>
+      </c>
+      <c r="K71" s="91">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="17" t="s">
         <v>49</v>
       </c>
@@ -4888,8 +5338,14 @@
       <c r="I72" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J72" s="80">
+        <v>0</v>
+      </c>
+      <c r="K72" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
         <v>50</v>
       </c>
@@ -4918,8 +5374,14 @@
       <c r="I73" s="81">
         <v>745476480000</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J73" s="81">
+        <v>745476480000</v>
+      </c>
+      <c r="K73" s="81">
+        <v>745476480000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
         <v>204</v>
       </c>
@@ -4948,8 +5410,14 @@
       <c r="I74" s="80">
         <v>100</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J74" s="80">
+        <v>100</v>
+      </c>
+      <c r="K74" s="80">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>414</v>
       </c>
@@ -4978,8 +5446,14 @@
       <c r="I75" s="80" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J75" s="80" t="s">
+        <v>86</v>
+      </c>
+      <c r="K75" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
         <v>400</v>
       </c>
@@ -5008,8 +5482,14 @@
       <c r="I76" s="89">
         <v>21600</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J76" s="89">
+        <v>21600</v>
+      </c>
+      <c r="K76" s="89">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
         <v>410</v>
       </c>
@@ -5038,8 +5518,14 @@
       <c r="I77" s="80">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J77" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="K77" s="80">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="35" t="s">
         <v>401</v>
       </c>
@@ -5068,8 +5554,14 @@
       <c r="I78" s="89">
         <v>60479.999999999993</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J78" s="89">
+        <v>60479.999999999993</v>
+      </c>
+      <c r="K78" s="89">
+        <v>60479.999999999993</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="35" t="s">
         <v>411</v>
       </c>
@@ -5098,8 +5590,14 @@
       <c r="I79" s="80">
         <v>0.85</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J79" s="80">
+        <v>0.85</v>
+      </c>
+      <c r="K79" s="80">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="35" t="s">
         <v>402</v>
       </c>
@@ -5128,8 +5626,14 @@
       <c r="I80" s="80">
         <v>518400</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J80" s="80">
+        <v>518400</v>
+      </c>
+      <c r="K80" s="80">
+        <v>518400</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="35" t="s">
         <v>412</v>
       </c>
@@ -5158,8 +5662,14 @@
       <c r="I81" s="80">
         <v>5184000</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J81" s="80">
+        <v>5184000</v>
+      </c>
+      <c r="K81" s="80">
+        <v>5184000</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="17" t="s">
         <v>51</v>
       </c>
@@ -5188,8 +5698,14 @@
       <c r="I82" s="90">
         <v>50000</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J82" s="90">
+        <v>50000</v>
+      </c>
+      <c r="K82" s="90">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="17" t="s">
         <v>52</v>
       </c>
@@ -5218,8 +5734,14 @@
       <c r="I83" s="80">
         <v>140000</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J83" s="80">
+        <v>140000</v>
+      </c>
+      <c r="K83" s="80">
+        <v>140000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="17" t="s">
         <v>53</v>
       </c>
@@ -5248,8 +5770,14 @@
       <c r="I84" s="81">
         <v>3.6636136999999999E-2</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J84" s="81">
+        <v>3.6636136999999999E-2</v>
+      </c>
+      <c r="K84" s="81">
+        <v>3.6636136999999999E-2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="17" t="s">
         <v>54</v>
       </c>
@@ -5278,8 +5806,14 @@
       <c r="I85" s="80">
         <v>4.4999999999999997E-3</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J85" s="80">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="K85" s="80">
+        <v>4.4999999999999997E-3</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="17" t="s">
         <v>55</v>
       </c>
@@ -5308,8 +5842,14 @@
       <c r="I86" s="80">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86" s="80">
+        <v>0.05</v>
+      </c>
+      <c r="K86" s="80">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="19" t="s">
         <v>213</v>
       </c>
@@ -5338,8 +5878,14 @@
       <c r="I87" s="80">
         <v>6.0000000000000002E-6</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J87" s="80">
+        <v>6.0000000000000002E-6</v>
+      </c>
+      <c r="K87" s="80">
+        <v>6.0000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
         <v>214</v>
       </c>
@@ -5368,8 +5914,14 @@
       <c r="I88" s="80">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88" s="80">
+        <v>1E-3</v>
+      </c>
+      <c r="K88" s="80">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>215</v>
       </c>
@@ -5398,8 +5950,14 @@
       <c r="I89" s="80">
         <v>374999999.99999994</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89" s="80">
+        <v>374999999.99999994</v>
+      </c>
+      <c r="K89" s="80">
+        <v>374999999.99999994</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="19" t="s">
         <v>216</v>
       </c>
@@ -5428,8 +5986,14 @@
       <c r="I90" s="81">
         <v>3.7037037037037038E-3</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90" s="81">
+        <v>3.7037037037037038E-3</v>
+      </c>
+      <c r="K90" s="81">
+        <v>3.7037037037037038E-3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="19" t="s">
         <v>217</v>
       </c>
@@ -5458,8 +6022,14 @@
       <c r="I91" s="80">
         <v>165600</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J91" s="80">
+        <v>165600</v>
+      </c>
+      <c r="K91" s="80">
+        <v>165600</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="13" t="s">
         <v>60</v>
       </c>
@@ -5488,8 +6058,14 @@
       <c r="I92" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92" s="80">
+        <v>20</v>
+      </c>
+      <c r="K92" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="13" t="s">
         <v>208</v>
       </c>
@@ -5518,8 +6094,14 @@
       <c r="I93" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93" s="80">
+        <v>1</v>
+      </c>
+      <c r="K93" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="13" t="s">
         <v>59</v>
       </c>
@@ -5548,8 +6130,14 @@
       <c r="I94" s="80">
         <v>21</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J94" s="80">
+        <v>21</v>
+      </c>
+      <c r="K94" s="80">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="23" t="s">
         <v>65</v>
       </c>
@@ -5578,8 +6166,14 @@
       <c r="I95" s="80">
         <v>0.64</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J95" s="80">
+        <v>0.64</v>
+      </c>
+      <c r="K95" s="80">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="23" t="s">
         <v>366</v>
       </c>
@@ -5608,8 +6202,14 @@
       <c r="I96" s="80">
         <v>8</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J96" s="80">
+        <v>8</v>
+      </c>
+      <c r="K96" s="80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="23" t="s">
         <v>367</v>
       </c>
@@ -5638,8 +6238,14 @@
       <c r="I97" s="80">
         <v>10</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J97" s="80">
+        <v>10</v>
+      </c>
+      <c r="K97" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="23" t="s">
         <v>368</v>
       </c>
@@ -5668,8 +6274,14 @@
       <c r="I98" s="80">
         <v>8</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98" s="80">
+        <v>8</v>
+      </c>
+      <c r="K98" s="80">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="23" t="s">
         <v>383</v>
       </c>
@@ -5698,8 +6310,14 @@
       <c r="I99" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J99" s="80">
+        <v>1</v>
+      </c>
+      <c r="K99" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="23" t="s">
         <v>385</v>
       </c>
@@ -5728,8 +6346,14 @@
       <c r="I100" s="80">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J100" s="80">
+        <v>0.5</v>
+      </c>
+      <c r="K100" s="80">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="23" t="s">
         <v>387</v>
       </c>
@@ -5758,8 +6382,14 @@
       <c r="I101" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101" s="80">
+        <v>0</v>
+      </c>
+      <c r="K101" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="23" t="s">
         <v>389</v>
       </c>
@@ -5788,8 +6418,14 @@
       <c r="I102" s="85">
         <v>1589759.9999999998</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J102" s="85">
+        <v>1589759.9999999998</v>
+      </c>
+      <c r="K102" s="85">
+        <v>1589759.9999999998</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="23" t="s">
         <v>391</v>
       </c>
@@ -5818,8 +6454,14 @@
       <c r="I103" s="85">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J103" s="85">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="K103" s="85">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
         <v>393</v>
       </c>
@@ -5848,8 +6490,14 @@
       <c r="I104" s="85">
         <v>6171428.5714285718</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J104" s="85">
+        <v>6171428.5714285718</v>
+      </c>
+      <c r="K104" s="85">
+        <v>6171428.5714285718</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="23" t="s">
         <v>421</v>
       </c>
@@ -5878,8 +6526,14 @@
       <c r="I105" s="85">
         <v>100</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J105" s="85">
+        <v>100</v>
+      </c>
+      <c r="K105" s="85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
         <v>423</v>
       </c>
@@ -5908,8 +6562,14 @@
       <c r="I106" s="85">
         <v>280800</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J106" s="85">
+        <v>280800</v>
+      </c>
+      <c r="K106" s="85">
+        <v>280800</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
         <v>425</v>
       </c>
@@ -5938,8 +6598,14 @@
       <c r="I107" s="85">
         <v>1.2847222222222224E-5</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J107" s="85">
+        <v>1.2847222222222224E-5</v>
+      </c>
+      <c r="K107" s="85">
+        <v>1.2847222222222224E-5</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
         <v>427</v>
       </c>
@@ -5968,8 +6634,14 @@
       <c r="I108" s="85">
         <v>100</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J108" s="85">
+        <v>100</v>
+      </c>
+      <c r="K108" s="85">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
         <v>429</v>
       </c>
@@ -5998,8 +6670,14 @@
       <c r="I109" s="85">
         <v>459648</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J109" s="85">
+        <v>459648</v>
+      </c>
+      <c r="K109" s="85">
+        <v>459648</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="23" t="s">
         <v>431</v>
       </c>
@@ -6028,8 +6706,14 @@
       <c r="I110" s="85">
         <v>1.2847222222222224E-5</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J110" s="85">
+        <v>1.2847222222222224E-5</v>
+      </c>
+      <c r="K110" s="85">
+        <v>1.2847222222222224E-5</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="23" t="s">
         <v>395</v>
       </c>
@@ -6058,8 +6742,14 @@
       <c r="I111" s="85">
         <v>21600</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111" s="85">
+        <v>21600</v>
+      </c>
+      <c r="K111" s="85">
+        <v>21600</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="23" t="s">
         <v>397</v>
       </c>
@@ -6088,8 +6778,14 @@
       <c r="I112" s="92">
         <v>43200</v>
       </c>
-    </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J112" s="92">
+        <v>43200</v>
+      </c>
+      <c r="K112" s="92">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113" s="13" t="s">
         <v>61</v>
       </c>
@@ -6118,8 +6814,14 @@
       <c r="I113" s="80">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J113" s="80">
+        <v>0.8</v>
+      </c>
+      <c r="K113" s="80">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114" s="13" t="s">
         <v>62</v>
       </c>
@@ -6148,8 +6850,14 @@
       <c r="I114" s="81">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J114" s="81">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="K114" s="81">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115" s="13" t="s">
         <v>63</v>
       </c>
@@ -6178,8 +6886,14 @@
       <c r="I115" s="80">
         <v>5.7899999999999998E-7</v>
       </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J115" s="80">
+        <v>5.7899999999999998E-7</v>
+      </c>
+      <c r="K115" s="80">
+        <v>5.7899999999999998E-7</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116" s="13" t="s">
         <v>64</v>
       </c>
@@ -6208,8 +6922,14 @@
       <c r="I116" s="81">
         <v>2.0833333333333335E-4</v>
       </c>
-    </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J116" s="81">
+        <v>2.0833333333333335E-4</v>
+      </c>
+      <c r="K116" s="81">
+        <v>2.0833333333333335E-4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117" s="13" t="s">
         <v>452</v>
       </c>
@@ -6238,8 +6958,14 @@
       <c r="I117" s="81">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J117" s="81">
+        <v>0</v>
+      </c>
+      <c r="K117" s="81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118" s="13" t="s">
         <v>454</v>
       </c>
@@ -6268,8 +6994,14 @@
       <c r="I118" s="81">
         <v>0</v>
       </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J118" s="81">
+        <v>0</v>
+      </c>
+      <c r="K118" s="81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119" s="71" t="s">
         <v>444</v>
       </c>
@@ -6297,8 +7029,16 @@
         <f>H119</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J119" s="93">
+        <f>I119</f>
+        <v>0</v>
+      </c>
+      <c r="K119" s="93">
+        <f>J119</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120" s="71" t="s">
         <v>67</v>
       </c>
@@ -6323,11 +7063,19 @@
         <v>0</v>
       </c>
       <c r="I120" s="93">
-        <f t="shared" ref="I120:I121" si="3">H120</f>
+        <f t="shared" ref="I120:K121" si="3">H120</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J120" s="93">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K120" s="93">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121" s="71" t="s">
         <v>448</v>
       </c>
@@ -6357,8 +7105,16 @@
         <f t="shared" si="3"/>
         <v>False</v>
       </c>
-    </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J121" s="93" t="str">
+        <f t="shared" si="3"/>
+        <v>False</v>
+      </c>
+      <c r="K121" s="93" t="str">
+        <f t="shared" si="3"/>
+        <v>False</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122" s="21" t="s">
         <v>66</v>
       </c>
@@ -6387,11 +7143,17 @@
       <c r="I122" s="86">
         <v>0.05</v>
       </c>
-      <c r="J122" s="60">
+      <c r="J122" s="86">
+        <v>0.05</v>
+      </c>
+      <c r="K122" s="86">
+        <v>0.05</v>
+      </c>
+      <c r="L122" s="60">
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123" s="21" t="s">
         <v>441</v>
       </c>
@@ -6420,8 +7182,14 @@
       <c r="I123" s="86">
         <v>4.9999999999999999E-13</v>
       </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J123" s="86">
+        <v>4.9999999999999999E-13</v>
+      </c>
+      <c r="K123" s="86">
+        <v>4.9999999999999999E-13</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="21" t="s">
         <v>228</v>
       </c>
@@ -6450,8 +7218,14 @@
       <c r="I124" s="80">
         <v>10</v>
       </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J124" s="80">
+        <v>10</v>
+      </c>
+      <c r="K124" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125" s="21" t="s">
         <v>229</v>
       </c>
@@ -6480,8 +7254,14 @@
       <c r="I125" s="80">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J125" s="80">
+        <v>-0.04</v>
+      </c>
+      <c r="K125" s="80">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126" s="21" t="s">
         <v>230</v>
       </c>
@@ -6510,8 +7290,14 @@
       <c r="I126" s="80">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J126" s="80">
+        <v>2.9</v>
+      </c>
+      <c r="K126" s="80">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127" s="21" t="s">
         <v>231</v>
       </c>
@@ -6540,8 +7326,14 @@
       <c r="I127" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J127" s="80">
+        <v>1</v>
+      </c>
+      <c r="K127" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128" s="21" t="s">
         <v>68</v>
       </c>
@@ -6570,8 +7362,14 @@
       <c r="I128" s="83">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128" s="83">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="K128" s="83">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="21" t="s">
         <v>232</v>
       </c>
@@ -6600,8 +7398,14 @@
       <c r="I129" s="80">
         <v>10</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129" s="80">
+        <v>10</v>
+      </c>
+      <c r="K129" s="80">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="21" t="s">
         <v>233</v>
       </c>
@@ -6630,8 +7434,14 @@
       <c r="I130" s="80">
         <v>-0.04</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130" s="80">
+        <v>-0.04</v>
+      </c>
+      <c r="K130" s="80">
+        <v>-0.04</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="21" t="s">
         <v>234</v>
       </c>
@@ -6660,8 +7470,14 @@
       <c r="I131" s="80">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131" s="80">
+        <v>2.9</v>
+      </c>
+      <c r="K131" s="80">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="21" t="s">
         <v>235</v>
       </c>
@@ -6690,8 +7506,14 @@
       <c r="I132" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132" s="80">
+        <v>1</v>
+      </c>
+      <c r="K132" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="21" t="s">
         <v>69</v>
       </c>
@@ -6720,8 +7542,14 @@
       <c r="I133" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133" s="80">
+        <v>0</v>
+      </c>
+      <c r="K133" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="75" t="s">
         <v>70</v>
       </c>
@@ -6750,8 +7578,14 @@
       <c r="I134" s="83">
         <v>5.0000000000000004E-6</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J134" s="83">
+        <v>5.0000000000000004E-6</v>
+      </c>
+      <c r="K134" s="83">
+        <v>5.0000000000000004E-6</v>
+      </c>
+    </row>
+    <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="23" t="s">
         <v>56</v>
       </c>
@@ -6780,8 +7614,14 @@
       <c r="I135" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J135" s="80">
+        <v>0</v>
+      </c>
+      <c r="K135" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="23" t="s">
         <v>57</v>
       </c>
@@ -6810,8 +7650,14 @@
       <c r="I136" s="80">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J136" s="80">
+        <v>2E-3</v>
+      </c>
+      <c r="K136" s="80">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="23" t="s">
         <v>58</v>
       </c>
@@ -6840,8 +7686,14 @@
       <c r="I137" s="83">
         <v>3.9999999999999998E-6</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J137" s="83">
+        <v>3.9999999999999998E-6</v>
+      </c>
+      <c r="K137" s="83">
+        <v>3.9999999999999998E-6</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="23" t="s">
         <v>71</v>
       </c>
@@ -6870,8 +7722,14 @@
       <c r="I138" s="83">
         <v>3.7699999999999999E-10</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J138" s="83">
+        <v>3.7699999999999999E-10</v>
+      </c>
+      <c r="K138" s="83">
+        <v>3.7699999999999999E-10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="23" t="s">
         <v>236</v>
       </c>
@@ -6900,8 +7758,14 @@
       <c r="I139" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J139" s="80">
+        <v>20</v>
+      </c>
+      <c r="K139" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="23" t="s">
         <v>237</v>
       </c>
@@ -6930,8 +7794,14 @@
       <c r="I140" s="80">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140" s="80">
+        <v>-0.06</v>
+      </c>
+      <c r="K140" s="80">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="23" t="s">
         <v>238</v>
       </c>
@@ -6960,8 +7830,14 @@
       <c r="I141" s="80">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141" s="80">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="K141" s="80">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="23" t="s">
         <v>239</v>
       </c>
@@ -6990,8 +7866,14 @@
       <c r="I142" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J142" s="80">
+        <v>1</v>
+      </c>
+      <c r="K142" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="23" t="s">
         <v>72</v>
       </c>
@@ -7020,8 +7902,14 @@
       <c r="I143" s="83">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J143" s="83">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="K143" s="83">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
         <v>73</v>
       </c>
@@ -7050,8 +7938,14 @@
       <c r="I144" s="83">
         <v>5.8333333333333335E-9</v>
       </c>
-    </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J144" s="83">
+        <v>5.8333333333333335E-9</v>
+      </c>
+      <c r="K144" s="83">
+        <v>5.8333333333333335E-9</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
         <v>240</v>
       </c>
@@ -7080,8 +7974,14 @@
       <c r="I145" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="146" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J145" s="80">
+        <v>20</v>
+      </c>
+      <c r="K145" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
         <v>241</v>
       </c>
@@ -7110,8 +8010,14 @@
       <c r="I146" s="80">
         <v>-0.06</v>
       </c>
-    </row>
-    <row r="147" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J146" s="80">
+        <v>-0.06</v>
+      </c>
+      <c r="K146" s="80">
+        <v>-0.06</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
         <v>242</v>
       </c>
@@ -7140,8 +8046,14 @@
       <c r="I147" s="80">
         <v>0.89100000000000001</v>
       </c>
-    </row>
-    <row r="148" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J147" s="80">
+        <v>0.89100000000000001</v>
+      </c>
+      <c r="K147" s="80">
+        <v>0.89100000000000001</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
         <v>243</v>
       </c>
@@ -7170,8 +8082,14 @@
       <c r="I148" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="149" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J148" s="80">
+        <v>1</v>
+      </c>
+      <c r="K148" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
         <v>74</v>
       </c>
@@ -7200,8 +8118,14 @@
       <c r="I149" s="83">
         <v>4.0000000000000003E-5</v>
       </c>
-    </row>
-    <row r="150" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J149" s="83">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="K149" s="83">
+        <v>4.0000000000000003E-5</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="s">
         <v>75</v>
       </c>
@@ -7230,8 +8154,14 @@
       <c r="I150" s="86">
         <v>4.0000000000000001E-8</v>
       </c>
-    </row>
-    <row r="151" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J150" s="86">
+        <v>4.0000000000000001E-8</v>
+      </c>
+      <c r="K150" s="86">
+        <v>4.0000000000000001E-8</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="s">
         <v>218</v>
       </c>
@@ -7260,8 +8190,14 @@
       <c r="I151" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="152" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J151" s="80">
+        <v>20</v>
+      </c>
+      <c r="K151" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="s">
         <v>219</v>
       </c>
@@ -7290,8 +8226,14 @@
       <c r="I152" s="80">
         <v>-4.4200000000000003E-2</v>
       </c>
-    </row>
-    <row r="153" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J152" s="80">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+      <c r="K152" s="80">
+        <v>-4.4200000000000003E-2</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153" s="9" t="s">
         <v>220</v>
       </c>
@@ -7320,8 +8262,14 @@
       <c r="I153" s="80">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J153" s="80">
+        <v>1.55</v>
+      </c>
+      <c r="K153" s="80">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154" s="9" t="s">
         <v>221</v>
       </c>
@@ -7350,8 +8298,14 @@
       <c r="I154" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="155" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J154" s="80">
+        <v>1</v>
+      </c>
+      <c r="K154" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155" s="9" t="s">
         <v>76</v>
       </c>
@@ -7380,8 +8334,14 @@
       <c r="I155" s="80">
         <v>2.7799999999999998E-4</v>
       </c>
-    </row>
-    <row r="156" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J155" s="80">
+        <v>2.7799999999999998E-4</v>
+      </c>
+      <c r="K155" s="80">
+        <v>2.7799999999999998E-4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156" s="25" t="s">
         <v>78</v>
       </c>
@@ -7412,11 +8372,19 @@
         <v>5.0000000000000005E-12</v>
       </c>
       <c r="J156" s="87">
+        <f>0.00000001/2000</f>
+        <v>5.0000000000000005E-12</v>
+      </c>
+      <c r="K156" s="87">
+        <f>0.00000001/2000</f>
+        <v>5.0000000000000005E-12</v>
+      </c>
+      <c r="L156" s="87">
         <f>0.0000001/2000</f>
         <v>4.9999999999999995E-11</v>
       </c>
     </row>
-    <row r="157" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157" s="25" t="s">
         <v>245</v>
       </c>
@@ -7445,8 +8413,14 @@
       <c r="I157" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="158" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J157" s="80">
+        <v>20</v>
+      </c>
+      <c r="K157" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158" s="25" t="s">
         <v>246</v>
       </c>
@@ -7475,8 +8449,14 @@
       <c r="I158" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="159" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J158" s="80">
+        <v>0</v>
+      </c>
+      <c r="K158" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159" s="25" t="s">
         <v>247</v>
       </c>
@@ -7505,8 +8485,14 @@
       <c r="I159" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="160" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J159" s="80">
+        <v>1</v>
+      </c>
+      <c r="K159" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160" s="25" t="s">
         <v>248</v>
       </c>
@@ -7535,8 +8521,14 @@
       <c r="I160" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J160" s="80">
+        <v>0</v>
+      </c>
+      <c r="K160" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="25" t="s">
         <v>79</v>
       </c>
@@ -7565,8 +8557,14 @@
       <c r="I161" s="80">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J161" s="80">
+        <v>0.4</v>
+      </c>
+      <c r="K161" s="80">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="33" t="s">
         <v>80</v>
       </c>
@@ -7595,8 +8593,14 @@
       <c r="I162" s="90">
         <v>2.0000000000000001E-9</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J162" s="90">
+        <v>2.0000000000000001E-9</v>
+      </c>
+      <c r="K162" s="90">
+        <v>2.0000000000000001E-9</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="33" t="s">
         <v>249</v>
       </c>
@@ -7625,8 +8629,14 @@
       <c r="I163" s="80">
         <v>25</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J163" s="80">
+        <v>25</v>
+      </c>
+      <c r="K163" s="80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="33" t="s">
         <v>250</v>
       </c>
@@ -7655,8 +8665,14 @@
       <c r="I164" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J164" s="80">
+        <v>0</v>
+      </c>
+      <c r="K164" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="33" t="s">
         <v>251</v>
       </c>
@@ -7685,8 +8701,14 @@
       <c r="I165" s="80">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J165" s="80">
+        <v>3.98</v>
+      </c>
+      <c r="K165" s="80">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="33" t="s">
         <v>252</v>
       </c>
@@ -7715,8 +8737,14 @@
       <c r="I166" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J166" s="80">
+        <v>1</v>
+      </c>
+      <c r="K166" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="33" t="s">
         <v>81</v>
       </c>
@@ -7745,8 +8773,14 @@
       <c r="I167" s="81">
         <v>1.6666666666666666E-4</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J167" s="81">
+        <v>1.6666666666666666E-4</v>
+      </c>
+      <c r="K167" s="81">
+        <v>1.6666666666666666E-4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="11" t="s">
         <v>253</v>
       </c>
@@ -7775,8 +8809,14 @@
       <c r="I168" s="83">
         <v>1E-8</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J168" s="83">
+        <v>1E-8</v>
+      </c>
+      <c r="K168" s="83">
+        <v>1E-8</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="11" t="s">
         <v>254</v>
       </c>
@@ -7805,8 +8845,14 @@
       <c r="I169" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J169" s="80">
+        <v>20</v>
+      </c>
+      <c r="K169" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="11" t="s">
         <v>255</v>
       </c>
@@ -7835,8 +8881,14 @@
       <c r="I170" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J170" s="80">
+        <v>0</v>
+      </c>
+      <c r="K170" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="11" t="s">
         <v>256</v>
       </c>
@@ -7865,8 +8917,14 @@
       <c r="I171" s="80">
         <v>2</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J171" s="80">
+        <v>2</v>
+      </c>
+      <c r="K171" s="80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="11" t="s">
         <v>257</v>
       </c>
@@ -7895,8 +8953,14 @@
       <c r="I172" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J172" s="80">
+        <v>1</v>
+      </c>
+      <c r="K172" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="11" t="s">
         <v>258</v>
       </c>
@@ -7925,8 +8989,14 @@
       <c r="I173" s="81">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J173" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="K173" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="11" t="s">
         <v>259</v>
       </c>
@@ -7955,8 +9025,14 @@
       <c r="I174" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J174" s="80">
+        <v>1</v>
+      </c>
+      <c r="K174" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="27" t="s">
         <v>260</v>
       </c>
@@ -7985,8 +9061,14 @@
       <c r="I175" s="80">
         <v>2.3533050791148899E-8</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J175" s="80">
+        <v>2.3533050791148899E-8</v>
+      </c>
+      <c r="K175" s="80">
+        <v>2.3533050791148899E-8</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="27" t="s">
         <v>261</v>
       </c>
@@ -8015,8 +9097,14 @@
       <c r="I176" s="80">
         <v>20</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J176" s="80">
+        <v>20</v>
+      </c>
+      <c r="K176" s="80">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="27" t="s">
         <v>262</v>
       </c>
@@ -8045,8 +9133,14 @@
       <c r="I177" s="80">
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J177" s="80">
+        <v>-0.187</v>
+      </c>
+      <c r="K177" s="80">
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="27" t="s">
         <v>263</v>
       </c>
@@ -8075,8 +9169,14 @@
       <c r="I178" s="80">
         <v>2.48</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J178" s="80">
+        <v>2.48</v>
+      </c>
+      <c r="K178" s="80">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="27" t="s">
         <v>264</v>
       </c>
@@ -8105,8 +9205,14 @@
       <c r="I179" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179" s="80">
+        <v>1</v>
+      </c>
+      <c r="K179" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="27" t="s">
         <v>265</v>
       </c>
@@ -8135,8 +9241,14 @@
       <c r="I180" s="80">
         <v>6.1060227588121015E-4</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J180" s="80">
+        <v>6.1060227588121015E-4</v>
+      </c>
+      <c r="K180" s="80">
+        <v>6.1060227588121015E-4</v>
+      </c>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="23" t="s">
         <v>266</v>
       </c>
@@ -8165,8 +9277,14 @@
       <c r="I181" s="89">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181" s="89">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="K181" s="89">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="23" t="s">
         <v>267</v>
       </c>
@@ -8195,8 +9313,14 @@
       <c r="I182" s="80">
         <v>25</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J182" s="80">
+        <v>25</v>
+      </c>
+      <c r="K182" s="80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="23" t="s">
         <v>268</v>
       </c>
@@ -8225,8 +9349,14 @@
       <c r="I183" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J183" s="80">
+        <v>0</v>
+      </c>
+      <c r="K183" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="23" t="s">
         <v>269</v>
       </c>
@@ -8255,8 +9385,14 @@
       <c r="I184" s="80">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184" s="80">
+        <v>3.98</v>
+      </c>
+      <c r="K184" s="80">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="23" t="s">
         <v>270</v>
       </c>
@@ -8285,8 +9421,14 @@
       <c r="I185" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J185" s="80">
+        <v>1</v>
+      </c>
+      <c r="K185" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="23" t="s">
         <v>271</v>
       </c>
@@ -8315,8 +9457,14 @@
       <c r="I186" s="81">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J186" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="K186" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="7" t="s">
         <v>272</v>
       </c>
@@ -8345,8 +9493,14 @@
       <c r="I187" s="89">
         <v>3.9999999999999998E-7</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J187" s="89">
+        <v>3.9999999999999998E-7</v>
+      </c>
+      <c r="K187" s="89">
+        <v>3.9999999999999998E-7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>273</v>
       </c>
@@ -8375,8 +9529,14 @@
       <c r="I188" s="80">
         <v>25</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J188" s="80">
+        <v>25</v>
+      </c>
+      <c r="K188" s="80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>274</v>
       </c>
@@ -8405,8 +9565,14 @@
       <c r="I189" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J189" s="80">
+        <v>0</v>
+      </c>
+      <c r="K189" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>275</v>
       </c>
@@ -8435,8 +9601,14 @@
       <c r="I190" s="80">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J190" s="80">
+        <v>3.98</v>
+      </c>
+      <c r="K190" s="80">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>276</v>
       </c>
@@ -8465,8 +9637,14 @@
       <c r="I191" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J191" s="80">
+        <v>1</v>
+      </c>
+      <c r="K191" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>277</v>
       </c>
@@ -8495,8 +9673,14 @@
       <c r="I192" s="81">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J192" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="K192" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="29" t="s">
         <v>278</v>
       </c>
@@ -8525,8 +9709,14 @@
       <c r="I193" s="89">
         <v>1.9999999999999999E-7</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J193" s="89">
+        <v>1.9999999999999999E-7</v>
+      </c>
+      <c r="K193" s="89">
+        <v>1.9999999999999999E-7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="29" t="s">
         <v>279</v>
       </c>
@@ -8555,8 +9745,14 @@
       <c r="I194" s="80">
         <v>25</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194" s="80">
+        <v>25</v>
+      </c>
+      <c r="K194" s="80">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="29" t="s">
         <v>280</v>
       </c>
@@ -8585,8 +9781,14 @@
       <c r="I195" s="80">
         <v>0</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J195" s="80">
+        <v>0</v>
+      </c>
+      <c r="K195" s="80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="29" t="s">
         <v>281</v>
       </c>
@@ -8615,8 +9817,14 @@
       <c r="I196" s="80">
         <v>3.98</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J196" s="80">
+        <v>3.98</v>
+      </c>
+      <c r="K196" s="80">
+        <v>3.98</v>
+      </c>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="29" t="s">
         <v>282</v>
       </c>
@@ -8645,8 +9853,14 @@
       <c r="I197" s="80">
         <v>1</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197" s="80">
+        <v>1</v>
+      </c>
+      <c r="K197" s="80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="29" t="s">
         <v>283</v>
       </c>
@@ -8675,39 +9889,51 @@
       <c r="I198" s="81">
         <v>8.3333333333333331E-5</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="31" t="s">
+      <c r="J198" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+      <c r="K198" s="81">
+        <v>8.3333333333333331E-5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A199" s="95" t="s">
         <v>361</v>
       </c>
-      <c r="B199" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="C199" s="3" t="s">
-        <v>489</v>
-      </c>
-      <c r="D199" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="E199" s="32" t="s">
+      <c r="B199" s="96" t="s">
+        <v>474</v>
+      </c>
+      <c r="C199" s="96" t="s">
+        <v>489</v>
+      </c>
+      <c r="D199" s="96" t="s">
+        <v>491</v>
+      </c>
+      <c r="E199" s="97" t="s">
         <v>203</v>
       </c>
-      <c r="F199" s="32" t="s">
+      <c r="F199" s="97" t="s">
         <v>91</v>
       </c>
-      <c r="G199" s="39" t="s">
+      <c r="G199" s="98" t="s">
         <v>89</v>
       </c>
-      <c r="H199" s="88" t="str">
+      <c r="H199" s="99" t="str">
         <f t="shared" si="5"/>
         <v>WHEAT</v>
       </c>
-      <c r="I199" s="83" t="s">
+      <c r="I199" s="100" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="97" t="s">
+      <c r="J199" s="100" t="s">
+        <v>89</v>
+      </c>
+      <c r="K199" s="100" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="200" spans="1:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="31" t="s">
         <v>493</v>
       </c>
       <c r="B200" s="3" t="s">
@@ -8719,57 +9945,71 @@
       <c r="D200" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="E200" s="98" t="s">
+      <c r="E200" s="32" t="s">
         <v>494</v>
       </c>
-      <c r="F200" s="98" t="s">
+      <c r="F200" s="32" t="s">
         <v>495</v>
       </c>
-      <c r="G200" s="99">
+      <c r="G200" s="39">
         <f>0.84*(0.36*0.36)</f>
         <v>0.10886399999999999</v>
       </c>
-      <c r="H200" s="100">
+      <c r="H200" s="88">
         <f>G200</f>
         <v>0.10886399999999999</v>
       </c>
-      <c r="I200" s="101">
+      <c r="I200" s="83">
         <f>H200</f>
         <v>0.10886399999999999</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" s="1" t="s">
+      <c r="J200" s="83">
+        <f>I200</f>
+        <v>0.10886399999999999</v>
+      </c>
+      <c r="K200" s="83">
+        <f>J200</f>
+        <v>0.10886399999999999</v>
+      </c>
+    </row>
+    <row r="201" spans="1:11" s="101" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
         <v>485</v>
       </c>
-      <c r="B201" s="1" t="s">
-        <v>474</v>
-      </c>
-      <c r="C201" s="1" t="s">
+      <c r="B201" s="2" t="s">
+        <v>474</v>
+      </c>
+      <c r="C201" s="2" t="s">
         <v>486</v>
       </c>
-      <c r="D201" s="1" t="s">
+      <c r="D201" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="E201" s="94" t="s">
+      <c r="E201" s="30" t="s">
         <v>487</v>
       </c>
-      <c r="F201" s="94" t="s">
+      <c r="F201" s="30" t="s">
         <v>488</v>
       </c>
-      <c r="G201" s="95">
+      <c r="G201" s="102">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="H201" s="95">
+      <c r="H201" s="102">
         <f>G201</f>
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="I201" s="96">
+      <c r="I201" s="103">
         <v>9.9999999999999995E-8</v>
       </c>
+      <c r="J201" s="104">
+        <v>4.9999999999999998E-7</v>
+      </c>
+      <c r="K201" s="104">
+        <v>3.9999999999999998E-7</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="I117:I118">
+  <conditionalFormatting sqref="I117:K118">
     <cfRule type="colorScale" priority="220">
       <colorScale>
         <cfvo type="min"/>
@@ -8781,7 +10021,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I122">
+  <conditionalFormatting sqref="I122:K122">
     <cfRule type="colorScale" priority="216">
       <colorScale>
         <cfvo type="min"/>
@@ -8803,7 +10043,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I123">
+  <conditionalFormatting sqref="I123:K123">
     <cfRule type="colorScale" priority="215">
       <colorScale>
         <cfvo type="min"/>
@@ -8825,7 +10065,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I128">
+  <conditionalFormatting sqref="I128:K128">
     <cfRule type="colorScale" priority="213">
       <colorScale>
         <cfvo type="min"/>
@@ -8837,7 +10077,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I134">
+  <conditionalFormatting sqref="I134:K134">
     <cfRule type="colorScale" priority="214">
       <colorScale>
         <cfvo type="min"/>
@@ -8869,7 +10109,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I150">
+  <conditionalFormatting sqref="I150:K150">
     <cfRule type="colorScale" priority="212">
       <colorScale>
         <cfvo type="min"/>
@@ -8901,7 +10141,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I156:J156">
+  <conditionalFormatting sqref="I156:L156">
     <cfRule type="colorScale" priority="211">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
added a condition for initial Unloading diffusion when shoot phloem concentrations were at 0.
</commit_message>
<xml_diff>
--- a/test/inputs/Scenarios.xlsx
+++ b/test/inputs/Scenarios.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\test\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CEF4D05-677F-4FC0-84BF-13A727FAB37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFEE2D9-3C39-4657-8595-E0F0C608E111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2196,7 +2196,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2408,7 +2408,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="11" fontId="16" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="16" fillId="50" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2733,11 +2732,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="7" ySplit="4" topLeftCell="H185" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="113" workbookViewId="0">
+      <pane xSplit="7" ySplit="4" topLeftCell="H191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J213" sqref="J213"/>
+      <selection pane="bottomRight" activeCell="L210" sqref="L210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2746,10 +2745,10 @@
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="16.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="12.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="56.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
     <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="27.42578125" style="40" customWidth="1"/>
-    <col min="8" max="8" width="45" style="40" customWidth="1"/>
+    <col min="7" max="7" width="11" style="40" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="40" customWidth="1"/>
     <col min="9" max="11" width="21.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10001,11 +10000,11 @@
       <c r="I201" s="103">
         <v>9.9999999999999995E-8</v>
       </c>
-      <c r="J201" s="104">
-        <v>4.9999999999999998E-7</v>
-      </c>
-      <c r="K201" s="104">
-        <v>3.9999999999999998E-7</v>
+      <c r="J201" s="103">
+        <v>1.1999999999999999E-7</v>
+      </c>
+      <c r="K201" s="103">
+        <v>1.4999999999999999E-7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>